<commit_message>
Finished London data exploration
</commit_message>
<xml_diff>
--- a/notebooks/CityNulls.xlsx
+++ b/notebooks/CityNulls.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="63">
   <si>
     <t>City</t>
   </si>
@@ -147,12 +147,6 @@
     <t>If summary field says Foggy then set cloudCover  to 1.0; otherwise set to 0.0</t>
   </si>
   <si>
-    <t>all nuls are when precipType = rain</t>
-  </si>
-  <si>
-    <t>all nuls are when precipType = rain; set nulls to 1.0</t>
-  </si>
-  <si>
     <t>for each station: replace null with averge of prior and subsetuqent non-null value for same station</t>
   </si>
   <si>
@@ -187,6 +181,36 @@
   </si>
   <si>
     <t>no holes; no problem</t>
+  </si>
+  <si>
+    <t>no values whatsoever</t>
+  </si>
+  <si>
+    <t>drop for London</t>
+  </si>
+  <si>
+    <t>no good values until 4/22 9:00pm</t>
+  </si>
+  <si>
+    <t>Station CD9 has an anoalous vlaue at 4/25 3pm. Replace with average of predecessor and successor</t>
+  </si>
+  <si>
+    <t>all values on 4/22 9pm and after ate fine.</t>
+  </si>
+  <si>
+    <t>BX9 CT2 KF1 MYZ TD5 should be dropped. Maybe drop CT3</t>
+  </si>
+  <si>
+    <t>BX9 CT2 TD5 should be dropped</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Replace with average of predecessor and successor</t>
+  </si>
+  <si>
+    <t>BX1 should be dropped</t>
+  </si>
+  <si>
+    <t>Station CD9 is anomalous</t>
   </si>
 </sst>
 </file>
@@ -1034,13 +1058,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19:I31"/>
+      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,7 +1076,7 @@
     <col min="5" max="5" width="11.08984375" customWidth="1"/>
     <col min="6" max="6" width="11.08984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="63.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="49.453125" style="1" customWidth="1"/>
     <col min="9" max="9" width="67.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1075,16 +1100,16 @@
         <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1104,16 +1129,16 @@
         <v>0.461596495497688</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1136,13 +1161,13 @@
         <v>-1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1165,13 +1190,13 @@
         <v>-1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1194,13 +1219,13 @@
         <v>-1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1223,13 +1248,13 @@
         <v>-100</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1252,13 +1277,13 @@
         <v>-1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1281,13 +1306,13 @@
         <v>-1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1310,13 +1335,13 @@
         <v>-100</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1342,7 +1367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1365,13 +1390,13 @@
         <v>-100</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1394,13 +1419,13 @@
         <v>-100</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1423,13 +1448,13 @@
         <v>-100</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1452,13 +1477,13 @@
         <v>-100</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1481,13 +1506,13 @@
         <v>-100</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1510,13 +1535,13 @@
         <v>-1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1539,13 +1564,13 @@
         <v>-100</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1568,13 +1593,13 @@
         <v>-5</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1594,13 +1619,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1620,13 +1645,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1646,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1672,13 +1697,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1698,13 +1723,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1724,13 +1749,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1750,13 +1775,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1776,13 +1801,13 @@
         <v>0</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1802,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1828,13 +1853,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1854,13 +1879,13 @@
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1880,13 +1905,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1906,10 +1931,10 @@
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1931,6 +1956,12 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
+      <c r="H32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -1951,6 +1982,12 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
+      <c r="H33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -1971,6 +2008,12 @@
       <c r="F34" s="1">
         <v>1</v>
       </c>
+      <c r="H34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -1991,6 +2034,15 @@
       <c r="F35" s="1">
         <v>0.44318477977586657</v>
       </c>
+      <c r="G35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -2011,6 +2063,15 @@
       <c r="F36" s="1">
         <v>0.44318477977586657</v>
       </c>
+      <c r="G36" s="2">
+        <v>-10</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -2031,6 +2092,15 @@
       <c r="F37" s="1">
         <v>0.43988358960993834</v>
       </c>
+      <c r="G37" s="2">
+        <v>-100</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -2051,8 +2121,14 @@
       <c r="F38" s="1">
         <v>0.43988358960993834</v>
       </c>
+      <c r="G38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="I38" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2074,8 +2150,14 @@
       <c r="F39" s="1">
         <v>0.43988358960993834</v>
       </c>
+      <c r="G39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="I39" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -2097,6 +2179,12 @@
       <c r="F40" s="1">
         <v>0.37837720441317002</v>
       </c>
+      <c r="G40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="I40" t="s">
         <v>39</v>
       </c>
@@ -2120,6 +2208,15 @@
       <c r="F41" s="1">
         <v>0.3178698636087221</v>
       </c>
+      <c r="G41" s="2">
+        <v>-100</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -2140,6 +2237,15 @@
       <c r="F42" s="1">
         <v>0.26296585874381029</v>
       </c>
+      <c r="G42" s="2">
+        <v>-100</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -2160,6 +2266,12 @@
       <c r="F43" s="1">
         <v>0.19138215619841889</v>
       </c>
+      <c r="G43" s="2">
+        <v>-100</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -2180,6 +2292,9 @@
       <c r="F44" s="1">
         <v>7.1974632959777601E-2</v>
       </c>
+      <c r="G44" s="2">
+        <v>-1</v>
+      </c>
       <c r="I44" t="s">
         <v>40</v>
       </c>
@@ -2203,8 +2318,14 @@
       <c r="F45" s="1">
         <v>5.6467726522456776E-4</v>
       </c>
-      <c r="I45" t="s">
-        <v>43</v>
+      <c r="G45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -2226,6 +2347,12 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
+      <c r="H46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -2246,6 +2373,12 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
+      <c r="H47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -2266,8 +2399,14 @@
       <c r="F48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -2286,8 +2425,14 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -2306,8 +2451,14 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2326,8 +2477,14 @@
       <c r="F51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -2346,8 +2503,14 @@
       <c r="F52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -2366,8 +2529,14 @@
       <c r="F53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -2386,8 +2555,14 @@
       <c r="F54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2406,8 +2581,14 @@
       <c r="F55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -2426,8 +2607,14 @@
       <c r="F56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H56" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -2446,8 +2633,14 @@
       <c r="F57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H57" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2466,8 +2659,14 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -2486,8 +2685,14 @@
       <c r="F59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H59" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -2506,8 +2711,14 @@
       <c r="F60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -2526,9 +2737,20 @@
       <c r="F61" s="1">
         <v>0</v>
       </c>
+      <c r="H61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I61">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="London"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:I61">
       <sortCondition ref="C2:C61"/>
     </sortState>

</xml_diff>